<commit_message>
PCA on last data from time series
</commit_message>
<xml_diff>
--- a/qualityoflife_country_compare_2021.xlsx
+++ b/qualityoflife_country_compare_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarogumulec/Documents/Kody/QualityOfLife/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90BCEA93-3A51-B941-A04C-8708DCB5D994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B60B2AB-4683-AA45-8541-03157BBE511D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="-28300" windowWidth="51200" windowHeight="28300" activeTab="3" xr2:uid="{72E829D7-3EE3-4F5A-80DA-9E2BC7D33FF7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="4" xr2:uid="{72E829D7-3EE3-4F5A-80DA-9E2BC7D33FF7}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -7817,7 +7817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC34AECA-0233-8F4D-9A6A-7C98DF6640BF}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="252" workbookViewId="0"/>
+    <sheetView zoomScale="143" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8305,8 +8305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{547C2114-F27E-BF47-8376-3AEAE43A1EC1}">
   <dimension ref="A1:C267"/>
   <sheetViews>
-    <sheetView zoomScale="173" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:C1"/>
+    <sheetView tabSelected="1" topLeftCell="A134" zoomScale="173" workbookViewId="0">
+      <selection activeCell="C139" sqref="C139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8439,9 +8439,6 @@
       <c r="B15" t="s">
         <v>191</v>
       </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -9270,9 +9267,6 @@
       <c r="B111" t="s">
         <v>369</v>
       </c>
-      <c r="C111">
-        <v>1</v>
-      </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
@@ -9327,9 +9321,6 @@
       <c r="B117" t="s">
         <v>380</v>
       </c>
-      <c r="C117">
-        <v>1</v>
-      </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
@@ -9425,7 +9416,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>401</v>
       </c>
@@ -9433,7 +9424,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>403</v>
       </c>
@@ -9441,7 +9432,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>405</v>
       </c>
@@ -9449,7 +9440,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>407</v>
       </c>
@@ -9457,7 +9448,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>409</v>
       </c>
@@ -9465,7 +9456,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>411</v>
       </c>
@@ -9473,7 +9464,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>413</v>
       </c>
@@ -9481,7 +9472,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>415</v>
       </c>
@@ -9489,7 +9480,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>417</v>
       </c>
@@ -9497,7 +9488,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>419</v>
       </c>
@@ -9505,18 +9496,15 @@
         <v>420</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>421</v>
       </c>
       <c r="B139" t="s">
         <v>422</v>
       </c>
-      <c r="C139">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>423</v>
       </c>
@@ -9524,7 +9512,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>425</v>
       </c>
@@ -9532,7 +9520,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>427</v>
       </c>
@@ -9540,7 +9528,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>429</v>
       </c>
@@ -9548,7 +9536,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>431</v>
       </c>
@@ -9702,9 +9690,6 @@
       </c>
       <c r="B161" t="s">
         <v>464</v>
-      </c>
-      <c r="C161">
-        <v>1</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
time dependence directionality+stability test
</commit_message>
<xml_diff>
--- a/qualityoflife_country_compare_2021.xlsx
+++ b/qualityoflife_country_compare_2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarogumulec/Documents/Kody/QualityOfLife/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{734BBB4A-27F4-5040-B9AC-F9BA0BA69BD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32235987-8BDE-EB49-BCDE-9AE2FC55D2B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="4" xr2:uid="{72E829D7-3EE3-4F5A-80DA-9E2BC7D33FF7}"/>
   </bookViews>
@@ -8545,8 +8545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{547C2114-F27E-BF47-8376-3AEAE43A1EC1}">
   <dimension ref="A1:C267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="173" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="173" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10219,7 +10219,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>504</v>
       </c>
@@ -10227,7 +10227,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>506</v>
       </c>
@@ -10235,7 +10235,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>508</v>
       </c>
@@ -10243,7 +10243,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>510</v>
       </c>
@@ -10251,7 +10251,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>512</v>
       </c>
@@ -10259,7 +10259,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>514</v>
       </c>
@@ -10267,7 +10267,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>516</v>
       </c>
@@ -10275,7 +10275,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>518</v>
       </c>
@@ -10283,7 +10283,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>520</v>
       </c>
@@ -10291,7 +10291,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>523</v>
       </c>
@@ -10299,7 +10299,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>525</v>
       </c>
@@ -10307,7 +10307,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>527</v>
       </c>
@@ -10315,15 +10315,18 @@
         <v>528</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>48</v>
       </c>
       <c r="B205" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C205">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>530</v>
       </c>
@@ -10331,7 +10334,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>532</v>
       </c>
@@ -10339,7 +10342,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>534</v>
       </c>

</xml_diff>

<commit_message>
manual scraping, sports added
</commit_message>
<xml_diff>
--- a/qualityoflife_country_compare_2021.xlsx
+++ b/qualityoflife_country_compare_2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarogumulec/Documents/Kody/QualityOfLife/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32235987-8BDE-EB49-BCDE-9AE2FC55D2B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7284AD6B-D44F-5246-97B6-B393CDFD3504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="4" xr2:uid="{72E829D7-3EE3-4F5A-80DA-9E2BC7D33FF7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="3" xr2:uid="{72E829D7-3EE3-4F5A-80DA-9E2BC7D33FF7}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="689">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="758">
   <si>
     <t>Země</t>
   </si>
@@ -2105,13 +2105,220 @@
   </si>
   <si>
     <t>jen jeden rok - 2024</t>
+  </si>
+  <si>
+    <t>API_SL.EMP.SMGT.FE.ZS_DS2_en_excel_v2_2099.xls</t>
+  </si>
+  <si>
+    <t>https://data.worldbank.org/indicator/SL.EMP.SMGT.FE.ZS?most_recent_value_desc=true</t>
+  </si>
+  <si>
+    <t>jen poslední roky</t>
+  </si>
+  <si>
+    <t>Female share of employment in senior and middle management (%)</t>
+  </si>
+  <si>
+    <t>Female in management</t>
+  </si>
+  <si>
+    <t>Female in parliament</t>
+  </si>
+  <si>
+    <t>Proportion of seats held by women in national parliaments (%)</t>
+  </si>
+  <si>
+    <t>API_SG.GEN.PARL.ZS_DS2_en_excel_v2_129525.xls</t>
+  </si>
+  <si>
+    <t>https://data.worldbank.org/indicator/SG.GEN.PARL.ZS?most_recent_year_desc=false</t>
+  </si>
+  <si>
+    <t>Renewable energy consumption</t>
+  </si>
+  <si>
+    <t>Renewable energy consumption (% of total final energy consumption)</t>
+  </si>
+  <si>
+    <t>API_EG.FEC.RNEW.ZS_DS2_en_excel_v2_130319.xls</t>
+  </si>
+  <si>
+    <t>https://data.worldbank.org/indicator/EG.FEC.RNEW.ZS</t>
+  </si>
+  <si>
+    <t>Employment in agriculture (% of total employment) (modeled ILO estimate)</t>
+  </si>
+  <si>
+    <t>Employment in agriculture</t>
+  </si>
+  <si>
+    <t>API_SL.AGR.EMPL.ZS_DS2_en_excel_v2_125963.xls</t>
+  </si>
+  <si>
+    <t>https://data.worldbank.org/indicator/SL.AGR.EMPL.ZS</t>
+  </si>
+  <si>
+    <t>Employment in services</t>
+  </si>
+  <si>
+    <t>https://data.worldbank.org/indicator/SL.SRV.EMPL.ZS</t>
+  </si>
+  <si>
+    <t>API_SL.SRV.EMPL.ZS_DS2_en_excel_v2_2275.xls</t>
+  </si>
+  <si>
+    <t>Employment in services (% of total employment) (modeled ILO estimate)</t>
+  </si>
+  <si>
+    <t>Urban population (% of total population)</t>
+  </si>
+  <si>
+    <t>Urban population</t>
+  </si>
+  <si>
+    <t>API_SP.URB.TOTL.IN.ZS_DS2_en_excel_v2_130058.xls</t>
+  </si>
+  <si>
+    <t>https://data.worldbank.org/indicator/SP.URB.TOTL.IN.ZS</t>
+  </si>
+  <si>
+    <t>Rural population (% of total population)</t>
+  </si>
+  <si>
+    <t>Rural population</t>
+  </si>
+  <si>
+    <t>API_SP.RUR.TOTL.ZS_DS2_en_excel_v2_2765.xls</t>
+  </si>
+  <si>
+    <t>https://data.worldbank.org/indicator/SP.RUR.TOTL.ZS</t>
+  </si>
+  <si>
+    <t>Znečištění vzduchu PM2.5</t>
+  </si>
+  <si>
+    <t>Zaměstnanost v zemědělství</t>
+  </si>
+  <si>
+    <t>Zaměstnanost ve službách</t>
+  </si>
+  <si>
+    <t>Městská populace</t>
+  </si>
+  <si>
+    <t>Venkovská populace</t>
+  </si>
+  <si>
+    <t>PM2.5 air pollution, mean annual exposure (micrograms per cubic meter)</t>
+  </si>
+  <si>
+    <t>Air polution</t>
+  </si>
+  <si>
+    <t>ug/m2</t>
+  </si>
+  <si>
+    <t>https://data.worldbank.org/indicator/EN.ATM.PM25.MC.M3</t>
+  </si>
+  <si>
+    <t>API_EN.ATM.PM25.MC.M3_DS2_en_excel_v2_2779.xls</t>
+  </si>
+  <si>
+    <t>Mortality caused by road traffic injury (per 100,000 population)</t>
+  </si>
+  <si>
+    <t>1/100k</t>
+  </si>
+  <si>
+    <t>Traffic mortality</t>
+  </si>
+  <si>
+    <t>API_SH.STA.TRAF.P5_DS2_en_excel_v2_115069.xls</t>
+  </si>
+  <si>
+    <t>https://data.worldbank.org/indicator/SH.STA.TRAF.P5</t>
+  </si>
+  <si>
+    <t>Úmrtí při dopravních nehodách</t>
+  </si>
+  <si>
+    <t>https://www.oecd.org/en/publications/2024/06/society-at-a-glance-2024_08001b73/full-report/affordable-housing_1a2ec30f.html#indicator-d1e11728-0ee0a256aa</t>
+  </si>
+  <si>
+    <t>OECD</t>
+  </si>
+  <si>
+    <t>lx8iym.xlsx</t>
+  </si>
+  <si>
+    <t>Jen rok 2022</t>
+  </si>
+  <si>
+    <t>Housing in own property</t>
+  </si>
+  <si>
+    <t>World Equality Index</t>
+  </si>
+  <si>
+    <t>equaldex</t>
+  </si>
+  <si>
+    <t>https://www.equaldex.com/equality-index-api</t>
+  </si>
+  <si>
+    <t>jen posled rok</t>
+  </si>
+  <si>
+    <t>LGBT Legal index</t>
+  </si>
+  <si>
+    <t>LGBT Public Opinion index</t>
+  </si>
+  <si>
+    <t>LGBT Equality index</t>
+  </si>
+  <si>
+    <t>Money From Abroad</t>
+  </si>
+  <si>
+    <t>Personal remittances, received (% of GDP)</t>
+  </si>
+  <si>
+    <t>https://data.worldbank.org/indicator/BX.TRF.PWKR.DT.GD.ZS?view=map</t>
+  </si>
+  <si>
+    <t>API_BX.TRF.PWKR.DT.GD.ZS_DS2_en_excel_v2_129363.xls</t>
+  </si>
+  <si>
+    <t>Exports of goods and services (% of GDP)</t>
+  </si>
+  <si>
+    <t>Export</t>
+  </si>
+  <si>
+    <t>API_NE.EXP.GNFS.ZS_DS2_en_excel_v2_129765.xls</t>
+  </si>
+  <si>
+    <t>https://data.worldbank.org/indicator/NE.EXP.GNFS.ZS?view=map&amp;year=2024</t>
+  </si>
+  <si>
+    <t>Fertility</t>
+  </si>
+  <si>
+    <t>Fertility rate, total (births per woman)</t>
+  </si>
+  <si>
+    <t>https://data.worldbank.org/indicator/SP.DYN.TFRT.IN?most_recent_value_desc=false&amp;view=map&amp;year=2024</t>
+  </si>
+  <si>
+    <t>API_SP.DYN.TFRT.IN_DS2_en_excel_v2_130353.xls</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2141,8 +2348,22 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2152,6 +2373,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2169,7 +2396,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2187,6 +2414,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hypertextový odkaz" xfId="1" builtinId="8"/>
@@ -2505,10 +2737,10 @@
   <dimension ref="A1:AJ33"/>
   <sheetViews>
     <sheetView zoomScale="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T9" sqref="T9"/>
+      <selection pane="bottomRight" activeCell="AC1" sqref="AC1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2522,10 +2754,10 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="12" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -2543,19 +2775,19 @@
       <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="12" t="s">
         <v>35</v>
       </c>
       <c r="N1" s="1" t="s">
@@ -2567,13 +2799,13 @@
       <c r="P1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="12" t="s">
         <v>37</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="12" t="s">
         <v>50</v>
       </c>
       <c r="T1" s="1" t="s">
@@ -2597,10 +2829,10 @@
       <c r="Z1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="12" t="s">
         <v>62</v>
       </c>
       <c r="AC1" s="1" t="s">
@@ -2615,10 +2847,10 @@
       <c r="AF1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AG1" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AH1" s="12" t="s">
         <v>68</v>
       </c>
       <c r="AI1" s="1" t="s">
@@ -7905,10 +8137,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC34AECA-0233-8F4D-9A6A-7C98DF6640BF}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView zoomScale="143" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="143" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8529,6 +8761,398 @@
         <v>688</v>
       </c>
     </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
+        <v>693</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>692</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E23" s="7">
+        <v>2022</v>
+      </c>
+      <c r="F23" s="5">
+        <v>45937</v>
+      </c>
+      <c r="G23" t="s">
+        <v>689</v>
+      </c>
+      <c r="H23" t="s">
+        <v>690</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
+        <v>694</v>
+      </c>
+      <c r="B24" t="s">
+        <v>695</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E24" s="7">
+        <v>1997</v>
+      </c>
+      <c r="F24" s="5">
+        <v>45937</v>
+      </c>
+      <c r="G24" t="s">
+        <v>696</v>
+      </c>
+      <c r="H24" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>698</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>699</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E25" s="7">
+        <v>1990</v>
+      </c>
+      <c r="F25" s="5">
+        <v>45937</v>
+      </c>
+      <c r="G25" t="s">
+        <v>700</v>
+      </c>
+      <c r="H25" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="7" t="s">
+        <v>703</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>702</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E26" s="7">
+        <v>1991</v>
+      </c>
+      <c r="F26" s="5">
+        <v>45937</v>
+      </c>
+      <c r="G26" t="s">
+        <v>704</v>
+      </c>
+      <c r="H26" t="s">
+        <v>705</v>
+      </c>
+      <c r="I26" s="11" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="7" t="s">
+        <v>706</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>709</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E27" s="7">
+        <v>1991</v>
+      </c>
+      <c r="F27" s="5">
+        <v>45937</v>
+      </c>
+      <c r="G27" t="s">
+        <v>708</v>
+      </c>
+      <c r="H27" t="s">
+        <v>707</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="7" t="s">
+        <v>711</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>710</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E28" s="7">
+        <v>1960</v>
+      </c>
+      <c r="F28" s="5">
+        <v>45937</v>
+      </c>
+      <c r="G28" t="s">
+        <v>712</v>
+      </c>
+      <c r="H28" t="s">
+        <v>713</v>
+      </c>
+      <c r="I28" s="11" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="7" t="s">
+        <v>715</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>714</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E29" s="7">
+        <v>1960</v>
+      </c>
+      <c r="F29" s="5">
+        <v>45937</v>
+      </c>
+      <c r="G29" t="s">
+        <v>716</v>
+      </c>
+      <c r="H29" t="s">
+        <v>717</v>
+      </c>
+      <c r="I29" s="11" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="7" t="s">
+        <v>724</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>723</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>725</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E30" s="7">
+        <v>1990</v>
+      </c>
+      <c r="F30" s="5">
+        <v>45937</v>
+      </c>
+      <c r="G30" t="s">
+        <v>727</v>
+      </c>
+      <c r="H30" t="s">
+        <v>726</v>
+      </c>
+      <c r="I30" s="11" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="7" t="s">
+        <v>730</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>728</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>729</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E31" s="7">
+        <v>2000</v>
+      </c>
+      <c r="F31" s="5">
+        <v>45937</v>
+      </c>
+      <c r="G31" t="s">
+        <v>731</v>
+      </c>
+      <c r="H31" t="s">
+        <v>732</v>
+      </c>
+      <c r="I31" s="11" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="7" t="s">
+        <v>738</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>735</v>
+      </c>
+      <c r="E32" s="7">
+        <v>2022</v>
+      </c>
+      <c r="G32" t="s">
+        <v>736</v>
+      </c>
+      <c r="H32" t="s">
+        <v>734</v>
+      </c>
+      <c r="I32" s="11" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>745</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>739</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>740</v>
+      </c>
+      <c r="E34" s="7">
+        <v>2025</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>741</v>
+      </c>
+      <c r="I34" s="11" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>743</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>740</v>
+      </c>
+      <c r="E35" s="7">
+        <v>2025</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>741</v>
+      </c>
+      <c r="I35" s="11" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>744</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>740</v>
+      </c>
+      <c r="E36" s="7">
+        <v>2025</v>
+      </c>
+      <c r="H36" s="13" t="s">
+        <v>741</v>
+      </c>
+      <c r="I36" s="11" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>746</v>
+      </c>
+      <c r="B37" t="s">
+        <v>747</v>
+      </c>
+      <c r="C37" t="s">
+        <v>103</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F37" s="5">
+        <v>45937</v>
+      </c>
+      <c r="G37" t="s">
+        <v>749</v>
+      </c>
+      <c r="H37" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>751</v>
+      </c>
+      <c r="B38" t="s">
+        <v>750</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E38" s="7">
+        <v>1990</v>
+      </c>
+      <c r="F38" s="5">
+        <v>45937</v>
+      </c>
+      <c r="G38" t="s">
+        <v>752</v>
+      </c>
+      <c r="H38" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>754</v>
+      </c>
+      <c r="B39" t="s">
+        <v>755</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G39" t="s">
+        <v>757</v>
+      </c>
+      <c r="H39" t="s">
+        <v>756</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H18" r:id="rId1" xr:uid="{E6D44943-1570-5A4B-82B5-DF9B2F835086}"/>
@@ -8538,6 +9162,7 @@
     <hyperlink ref="H22" r:id="rId5" xr:uid="{9FCC0F3E-9A61-FF43-A4A2-857CEC99F442}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -8545,8 +9170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{547C2114-F27E-BF47-8376-3AEAE43A1EC1}">
   <dimension ref="A1:C267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="173" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView topLeftCell="A2" zoomScale="173" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8589,10 +9214,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>197</v>
+        <v>211</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -8600,10 +9225,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -8622,10 +9247,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -8644,10 +9269,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>349</v>
       </c>
       <c r="B9" t="s">
-        <v>233</v>
+        <v>350</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -8655,10 +9280,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -8666,10 +9291,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>271</v>
       </c>
       <c r="B11" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -8677,10 +9302,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>266</v>
+        <v>297</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -8688,10 +9313,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>271</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>272</v>
+        <v>304</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -8699,10 +9324,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>295</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>296</v>
+        <v>307</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -8710,10 +9335,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>316</v>
       </c>
       <c r="B15" t="s">
-        <v>297</v>
+        <v>317</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -8721,10 +9346,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>304</v>
+        <v>266</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -8732,10 +9357,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>307</v>
+        <v>330</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -8743,10 +9368,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>314</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>315</v>
+        <v>353</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -8754,10 +9379,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>316</v>
+        <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>317</v>
+        <v>238</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -8765,10 +9390,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>377</v>
       </c>
       <c r="B20" t="s">
-        <v>330</v>
+        <v>378</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -8776,10 +9401,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>349</v>
+        <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>350</v>
+        <v>372</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -8787,10 +9412,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B22" t="s">
-        <v>353</v>
+        <v>381</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -8798,10 +9423,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>372</v>
+        <v>386</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -8809,10 +9434,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>377</v>
+        <v>40</v>
       </c>
       <c r="B24" t="s">
-        <v>378</v>
+        <v>436</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -8820,10 +9445,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="B25" t="s">
-        <v>381</v>
+        <v>433</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -8831,10 +9456,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>14</v>
+        <v>445</v>
       </c>
       <c r="B26" t="s">
-        <v>386</v>
+        <v>446</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -8842,10 +9467,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>469</v>
       </c>
       <c r="B27" t="s">
-        <v>433</v>
+        <v>470</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -8853,18 +9478,21 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>434</v>
+        <v>39</v>
       </c>
       <c r="B28" t="s">
-        <v>435</v>
+        <v>497</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>436</v>
+        <v>503</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -8872,10 +9500,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>445</v>
+        <v>42</v>
       </c>
       <c r="B30" t="s">
-        <v>446</v>
+        <v>498</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -8883,10 +9511,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>469</v>
+        <v>20</v>
       </c>
       <c r="B31" t="s">
-        <v>470</v>
+        <v>522</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -8894,10 +9522,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B32" t="s">
-        <v>497</v>
+        <v>529</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -8905,10 +9533,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B33" t="s">
-        <v>498</v>
+        <v>542</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -8916,10 +9544,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>543</v>
       </c>
       <c r="B34" t="s">
-        <v>503</v>
+        <v>544</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -8927,10 +9555,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>20</v>
+        <v>567</v>
       </c>
       <c r="B35" t="s">
-        <v>522</v>
+        <v>568</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -8938,10 +9566,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>46</v>
+        <v>581</v>
       </c>
       <c r="B36" t="s">
-        <v>542</v>
+        <v>582</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -8949,10 +9577,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>543</v>
+        <v>22</v>
       </c>
       <c r="B37" t="s">
-        <v>544</v>
+        <v>583</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -8960,10 +9588,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>567</v>
+        <v>295</v>
       </c>
       <c r="B38" t="s">
-        <v>568</v>
+        <v>296</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -8971,10 +9599,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>581</v>
+        <v>23</v>
       </c>
       <c r="B39" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -8982,10 +9610,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B40" t="s">
-        <v>583</v>
+        <v>233</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -8993,10 +9621,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>23</v>
+        <v>625</v>
       </c>
       <c r="B41" t="s">
-        <v>584</v>
+        <v>626</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -9004,10 +9632,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>625</v>
+        <v>26</v>
       </c>
       <c r="B42" t="s">
-        <v>626</v>
+        <v>633</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -9015,10 +9643,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>26</v>
+        <v>314</v>
       </c>
       <c r="B43" t="s">
-        <v>633</v>
+        <v>315</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -9037,10 +9665,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="B45" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -9053,26 +9681,26 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B47" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>170</v>
+        <v>275</v>
       </c>
       <c r="B48" t="s">
-        <v>171</v>
+        <v>276</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="B49" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -9085,50 +9713,50 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B51" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="B52" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B53" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B54" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B55" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>188</v>
+        <v>164</v>
       </c>
       <c r="B56" t="s">
-        <v>189</v>
+        <v>165</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
@@ -9149,66 +9777,66 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>195</v>
+        <v>207</v>
       </c>
       <c r="B59" t="s">
-        <v>196</v>
+        <v>208</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="B60" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B61" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="B62" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="B63" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="B64" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B65" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="B66" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
@@ -9221,106 +9849,106 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="B68" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B69" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>222</v>
+        <v>645</v>
       </c>
       <c r="B70" t="s">
-        <v>223</v>
+        <v>646</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B71" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>226</v>
+        <v>200</v>
       </c>
       <c r="B72" t="s">
-        <v>227</v>
+        <v>201</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>228</v>
+        <v>195</v>
       </c>
       <c r="B73" t="s">
-        <v>229</v>
+        <v>196</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>231</v>
+        <v>251</v>
       </c>
       <c r="B74" t="s">
-        <v>232</v>
+        <v>252</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>234</v>
+        <v>393</v>
       </c>
       <c r="B75" t="s">
-        <v>235</v>
+        <v>394</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="B76" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>239</v>
+        <v>255</v>
       </c>
       <c r="B77" t="s">
-        <v>240</v>
+        <v>256</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>241</v>
+        <v>261</v>
       </c>
       <c r="B78" t="s">
-        <v>242</v>
+        <v>262</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="B79" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="B80" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
@@ -9341,50 +9969,50 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="B83" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="B84" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B85" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
       <c r="B86" t="s">
-        <v>258</v>
+        <v>240</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B87" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B88" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
@@ -9421,82 +10049,82 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="B93" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="B94" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B95" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>281</v>
+        <v>597</v>
       </c>
       <c r="B96" t="s">
-        <v>282</v>
+        <v>598</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="B97" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="B98" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>287</v>
+        <v>561</v>
       </c>
       <c r="B99" t="s">
-        <v>288</v>
+        <v>562</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>289</v>
+        <v>328</v>
       </c>
       <c r="B100" t="s">
-        <v>290</v>
+        <v>329</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B101" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>293</v>
+        <v>585</v>
       </c>
       <c r="B102" t="s">
-        <v>294</v>
+        <v>586</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
@@ -9509,106 +10137,106 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="B104" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>302</v>
+        <v>285</v>
       </c>
       <c r="B105" t="s">
-        <v>303</v>
+        <v>286</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>305</v>
+        <v>283</v>
       </c>
       <c r="B106" t="s">
-        <v>306</v>
+        <v>284</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>308</v>
+        <v>599</v>
       </c>
       <c r="B107" t="s">
-        <v>309</v>
+        <v>600</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="B108" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B109" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>318</v>
+        <v>305</v>
       </c>
       <c r="B110" t="s">
-        <v>319</v>
+        <v>306</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>320</v>
+        <v>302</v>
       </c>
       <c r="B111" t="s">
-        <v>321</v>
+        <v>303</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>322</v>
+        <v>538</v>
       </c>
       <c r="B112" t="s">
-        <v>323</v>
+        <v>539</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="B113" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B114" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="B115" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="B116" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
@@ -9621,10 +10249,10 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B118" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
@@ -9637,570 +10265,570 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B120" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>341</v>
+        <v>322</v>
       </c>
       <c r="B121" t="s">
-        <v>342</v>
+        <v>323</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>343</v>
+        <v>326</v>
       </c>
       <c r="B122" t="s">
-        <v>344</v>
+        <v>327</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="B123" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="B124" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B125" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>354</v>
+        <v>341</v>
       </c>
       <c r="B126" t="s">
-        <v>355</v>
+        <v>342</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>356</v>
+        <v>345</v>
       </c>
       <c r="B127" t="s">
-        <v>357</v>
+        <v>346</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>358</v>
+        <v>343</v>
       </c>
       <c r="B128" t="s">
-        <v>359</v>
+        <v>344</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>360</v>
+        <v>595</v>
       </c>
       <c r="B129" t="s">
-        <v>361</v>
+        <v>596</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>362</v>
+        <v>234</v>
       </c>
       <c r="B130" t="s">
-        <v>363</v>
+        <v>235</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>364</v>
+        <v>236</v>
       </c>
       <c r="B131" t="s">
-        <v>365</v>
+        <v>237</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>366</v>
+        <v>354</v>
       </c>
       <c r="B132" t="s">
-        <v>367</v>
+        <v>355</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>368</v>
+        <v>356</v>
       </c>
       <c r="B133" t="s">
-        <v>369</v>
+        <v>357</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="B134" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="B135" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>375</v>
+        <v>358</v>
       </c>
       <c r="B136" t="s">
-        <v>376</v>
+        <v>359</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>379</v>
+        <v>368</v>
       </c>
       <c r="B137" t="s">
-        <v>380</v>
+        <v>369</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>382</v>
+        <v>362</v>
       </c>
       <c r="B138" t="s">
-        <v>383</v>
+        <v>363</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
       <c r="B139" t="s">
-        <v>385</v>
+        <v>374</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>387</v>
+        <v>375</v>
       </c>
       <c r="B140" t="s">
-        <v>388</v>
+        <v>376</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>389</v>
+        <v>366</v>
       </c>
       <c r="B141" t="s">
-        <v>390</v>
+        <v>367</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>391</v>
+        <v>379</v>
       </c>
       <c r="B142" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>393</v>
+        <v>382</v>
       </c>
       <c r="B143" t="s">
-        <v>394</v>
+        <v>383</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>395</v>
+        <v>384</v>
       </c>
       <c r="B144" t="s">
-        <v>396</v>
+        <v>385</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>397</v>
+        <v>387</v>
       </c>
       <c r="B145" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>399</v>
+        <v>389</v>
       </c>
       <c r="B146" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="B147" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>403</v>
+        <v>527</v>
       </c>
       <c r="B148" t="s">
-        <v>404</v>
+        <v>528</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="B149" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>407</v>
+        <v>657</v>
       </c>
       <c r="B150" t="s">
-        <v>408</v>
+        <v>658</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="B151" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>411</v>
+        <v>391</v>
       </c>
       <c r="B152" t="s">
-        <v>412</v>
+        <v>392</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="B153" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>415</v>
+        <v>431</v>
       </c>
       <c r="B154" t="s">
-        <v>416</v>
+        <v>432</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B155" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>419</v>
+        <v>403</v>
       </c>
       <c r="B156" t="s">
-        <v>420</v>
+        <v>404</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>421</v>
+        <v>609</v>
       </c>
       <c r="B157" t="s">
-        <v>422</v>
+        <v>610</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="B158" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>425</v>
+        <v>407</v>
       </c>
       <c r="B159" t="s">
-        <v>426</v>
+        <v>408</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="B160" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>429</v>
+        <v>409</v>
       </c>
       <c r="B161" t="s">
-        <v>430</v>
+        <v>410</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>431</v>
+        <v>411</v>
       </c>
       <c r="B162" t="s">
-        <v>432</v>
+        <v>412</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>437</v>
+        <v>421</v>
       </c>
       <c r="B163" t="s">
-        <v>438</v>
+        <v>422</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>439</v>
+        <v>427</v>
       </c>
       <c r="B164" t="s">
-        <v>440</v>
+        <v>428</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>441</v>
+        <v>419</v>
       </c>
       <c r="B165" t="s">
-        <v>442</v>
+        <v>420</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>443</v>
+        <v>425</v>
       </c>
       <c r="B166" t="s">
-        <v>444</v>
+        <v>426</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>447</v>
+        <v>434</v>
       </c>
       <c r="B167" t="s">
-        <v>448</v>
+        <v>435</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>449</v>
+        <v>437</v>
       </c>
       <c r="B168" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="B169" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>453</v>
+        <v>481</v>
       </c>
       <c r="B170" t="s">
-        <v>454</v>
+        <v>482</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>455</v>
+        <v>483</v>
       </c>
       <c r="B171" t="s">
-        <v>456</v>
+        <v>484</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>457</v>
+        <v>449</v>
       </c>
       <c r="B172" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="B173" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="B174" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="B175" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>465</v>
+        <v>477</v>
       </c>
       <c r="B176" t="s">
-        <v>466</v>
+        <v>478</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>467</v>
+        <v>479</v>
       </c>
       <c r="B177" t="s">
-        <v>468</v>
+        <v>480</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>471</v>
+        <v>453</v>
       </c>
       <c r="B178" t="s">
-        <v>472</v>
+        <v>454</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>473</v>
+        <v>310</v>
       </c>
       <c r="B179" t="s">
-        <v>474</v>
+        <v>311</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>475</v>
+        <v>451</v>
       </c>
       <c r="B180" t="s">
-        <v>476</v>
+        <v>452</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>477</v>
+        <v>467</v>
       </c>
       <c r="B181" t="s">
-        <v>478</v>
+        <v>468</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>479</v>
+        <v>613</v>
       </c>
       <c r="B182" t="s">
-        <v>480</v>
+        <v>614</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>481</v>
+        <v>457</v>
       </c>
       <c r="B183" t="s">
-        <v>482</v>
+        <v>458</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>483</v>
+        <v>443</v>
       </c>
       <c r="B184" t="s">
-        <v>484</v>
+        <v>444</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>485</v>
+        <v>471</v>
       </c>
       <c r="B185" t="s">
-        <v>486</v>
+        <v>472</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>487</v>
+        <v>441</v>
       </c>
       <c r="B186" t="s">
-        <v>488</v>
+        <v>442</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>489</v>
+        <v>475</v>
       </c>
       <c r="B187" t="s">
-        <v>490</v>
+        <v>476</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>491</v>
+        <v>465</v>
       </c>
       <c r="B188" t="s">
-        <v>492</v>
+        <v>466</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="B189" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>495</v>
+        <v>501</v>
       </c>
       <c r="B190" t="s">
-        <v>496</v>
+        <v>502</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.2">
@@ -10213,597 +10841,594 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>501</v>
+        <v>489</v>
       </c>
       <c r="B192" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
+        <v>495</v>
+      </c>
+      <c r="B193" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>491</v>
+      </c>
+      <c r="B194" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>493</v>
+      </c>
+      <c r="B195" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>485</v>
+      </c>
+      <c r="B196" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>459</v>
+      </c>
+      <c r="B197" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>473</v>
+      </c>
+      <c r="B198" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>370</v>
+      </c>
+      <c r="B199" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
         <v>504</v>
       </c>
-      <c r="B193" t="s">
+      <c r="B200" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A194" t="s">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
         <v>506</v>
       </c>
-      <c r="B194" t="s">
+      <c r="B201" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A195" t="s">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
         <v>508</v>
       </c>
-      <c r="B195" t="s">
+      <c r="B202" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A196" t="s">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>534</v>
+      </c>
+      <c r="B203" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
         <v>510</v>
       </c>
-      <c r="B196" t="s">
+      <c r="B204" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A197" t="s">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
+        <v>518</v>
+      </c>
+      <c r="B205" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
         <v>512</v>
       </c>
-      <c r="B197" t="s">
+      <c r="B206" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A198" t="s">
-        <v>514</v>
-      </c>
-      <c r="B198" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A199" t="s">
-        <v>516</v>
-      </c>
-      <c r="B199" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A200" t="s">
-        <v>518</v>
-      </c>
-      <c r="B200" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A201" t="s">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
         <v>520</v>
       </c>
-      <c r="B201" t="s">
+      <c r="B207" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A202" t="s">
-        <v>523</v>
-      </c>
-      <c r="B202" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A203" t="s">
-        <v>525</v>
-      </c>
-      <c r="B203" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A204" t="s">
-        <v>527</v>
-      </c>
-      <c r="B204" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A205" t="s">
-        <v>48</v>
-      </c>
-      <c r="B205" t="s">
-        <v>529</v>
-      </c>
-      <c r="C205">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A206" t="s">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
         <v>530</v>
       </c>
-      <c r="B206" t="s">
+      <c r="B208" t="s">
         <v>531</v>
-      </c>
-    </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A207" t="s">
-        <v>532</v>
-      </c>
-      <c r="B207" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A208" t="s">
-        <v>534</v>
-      </c>
-      <c r="B208" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>536</v>
+        <v>514</v>
       </c>
       <c r="B209" t="s">
-        <v>537</v>
+        <v>515</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>538</v>
+        <v>516</v>
       </c>
       <c r="B210" t="s">
-        <v>539</v>
+        <v>517</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="B211" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>545</v>
+        <v>523</v>
       </c>
       <c r="B212" t="s">
-        <v>546</v>
+        <v>524</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>547</v>
+        <v>525</v>
       </c>
       <c r="B213" t="s">
-        <v>548</v>
+        <v>526</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>549</v>
+        <v>540</v>
       </c>
       <c r="B214" t="s">
-        <v>550</v>
+        <v>541</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="B215" t="s">
-        <v>552</v>
+        <v>546</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>553</v>
+        <v>655</v>
       </c>
       <c r="B216" t="s">
-        <v>554</v>
+        <v>656</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>555</v>
+        <v>563</v>
       </c>
       <c r="B217" t="s">
-        <v>556</v>
+        <v>564</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>557</v>
+        <v>577</v>
       </c>
       <c r="B218" t="s">
-        <v>558</v>
+        <v>578</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>559</v>
+        <v>549</v>
       </c>
       <c r="B219" t="s">
-        <v>560</v>
+        <v>550</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>561</v>
+        <v>553</v>
       </c>
       <c r="B220" t="s">
-        <v>562</v>
+        <v>554</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>563</v>
+        <v>589</v>
       </c>
       <c r="B221" t="s">
-        <v>564</v>
+        <v>590</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
       <c r="B222" t="s">
-        <v>566</v>
+        <v>560</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>569</v>
+        <v>555</v>
       </c>
       <c r="B223" t="s">
-        <v>570</v>
+        <v>556</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>571</v>
+        <v>587</v>
       </c>
       <c r="B224" t="s">
-        <v>572</v>
+        <v>588</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="B225" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>575</v>
+        <v>557</v>
       </c>
       <c r="B226" t="s">
-        <v>576</v>
+        <v>558</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>577</v>
+        <v>565</v>
       </c>
       <c r="B227" t="s">
-        <v>578</v>
+        <v>566</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>579</v>
+        <v>661</v>
       </c>
       <c r="B228" t="s">
-        <v>580</v>
+        <v>662</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>585</v>
+        <v>547</v>
       </c>
       <c r="B229" t="s">
-        <v>586</v>
+        <v>548</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>587</v>
+        <v>617</v>
       </c>
       <c r="B230" t="s">
-        <v>588</v>
+        <v>618</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>589</v>
+        <v>571</v>
       </c>
       <c r="B231" t="s">
-        <v>590</v>
+        <v>572</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>591</v>
+        <v>423</v>
       </c>
       <c r="B232" t="s">
-        <v>592</v>
+        <v>424</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>593</v>
+        <v>397</v>
       </c>
       <c r="B233" t="s">
-        <v>594</v>
+        <v>398</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>595</v>
+        <v>413</v>
       </c>
       <c r="B234" t="s">
-        <v>596</v>
+        <v>414</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>597</v>
+        <v>439</v>
       </c>
       <c r="B235" t="s">
-        <v>598</v>
+        <v>440</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>599</v>
+        <v>641</v>
       </c>
       <c r="B236" t="s">
-        <v>600</v>
+        <v>642</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>601</v>
+        <v>573</v>
       </c>
       <c r="B237" t="s">
-        <v>602</v>
+        <v>574</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>603</v>
+        <v>569</v>
       </c>
       <c r="B238" t="s">
-        <v>604</v>
+        <v>570</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>605</v>
+        <v>619</v>
       </c>
       <c r="B239" t="s">
-        <v>606</v>
+        <v>620</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>607</v>
+        <v>551</v>
       </c>
       <c r="B240" t="s">
-        <v>608</v>
+        <v>552</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>609</v>
+        <v>579</v>
       </c>
       <c r="B241" t="s">
-        <v>610</v>
+        <v>580</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>611</v>
+        <v>591</v>
       </c>
       <c r="B242" t="s">
-        <v>612</v>
+        <v>592</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
-        <v>613</v>
+        <v>605</v>
       </c>
       <c r="B243" t="s">
-        <v>614</v>
+        <v>606</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
-        <v>615</v>
+        <v>629</v>
       </c>
       <c r="B244" t="s">
-        <v>616</v>
+        <v>630</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>617</v>
+        <v>603</v>
       </c>
       <c r="B245" t="s">
-        <v>618</v>
+        <v>604</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>619</v>
+        <v>611</v>
       </c>
       <c r="B246" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>621</v>
+        <v>601</v>
       </c>
       <c r="B247" t="s">
-        <v>622</v>
+        <v>602</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>623</v>
+        <v>615</v>
       </c>
       <c r="B248" t="s">
-        <v>624</v>
+        <v>616</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="B249" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>629</v>
+        <v>623</v>
       </c>
       <c r="B250" t="s">
-        <v>630</v>
+        <v>624</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>631</v>
+        <v>607</v>
       </c>
       <c r="B251" t="s">
-        <v>632</v>
+        <v>608</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>634</v>
+        <v>593</v>
       </c>
       <c r="B252" t="s">
-        <v>635</v>
+        <v>594</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>636</v>
+        <v>627</v>
       </c>
       <c r="B253" t="s">
-        <v>637</v>
+        <v>628</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
-        <v>639</v>
+        <v>631</v>
       </c>
       <c r="B254" t="s">
-        <v>640</v>
+        <v>632</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
-        <v>641</v>
+        <v>180</v>
       </c>
       <c r="B255" t="s">
-        <v>642</v>
+        <v>181</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
-        <v>643</v>
+        <v>634</v>
       </c>
       <c r="B256" t="s">
-        <v>644</v>
+        <v>635</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>645</v>
+        <v>636</v>
       </c>
       <c r="B257" t="s">
-        <v>646</v>
+        <v>637</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>647</v>
+        <v>639</v>
       </c>
       <c r="B258" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="B259" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
       <c r="B260" t="s">
-        <v>652</v>
+        <v>644</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="B261" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
-        <v>655</v>
+        <v>647</v>
       </c>
       <c r="B262" t="s">
-        <v>656</v>
+        <v>648</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
-        <v>657</v>
+        <v>532</v>
       </c>
       <c r="B263" t="s">
-        <v>658</v>
+        <v>533</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
-        <v>659</v>
+        <v>653</v>
       </c>
       <c r="B264" t="s">
-        <v>660</v>
+        <v>654</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="B265" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.2">
@@ -10823,8 +11448,9 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C267">
-    <sortCondition ref="C2:C267"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C268">
+    <sortCondition ref="C2:C268"/>
+    <sortCondition ref="A2:A268"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>